<commit_message>
NS demo prep changes, to not loose
</commit_message>
<xml_diff>
--- a/ns-dmd/Base Data Model-NS.xlsx
+++ b/ns-dmd/Base Data Model-NS.xlsx
@@ -31,7 +31,7 @@
     <definedName name="_Attribute_Name">'[1]S7 - Attribute'!$E$2:$E$1048576</definedName>
     <definedName name="_Boolean">[1]!Boolean[Boolean]</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ATTRIBUTES!$A$1:$V$436</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$Z$918</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$Z$909</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
     <definedName name="_RefDataAttribute">ATTRIBUTES!#REF!</definedName>
     <definedName name="RefDataAttribute">ATTRIBUTES!#REF!</definedName>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7101" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7060" uniqueCount="1147">
   <si>
     <t>ACTION</t>
   </si>
@@ -3563,6 +3563,9 @@
   </si>
   <si>
     <t>linktomasterversion</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -4394,11 +4397,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4513,33 +4516,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>606</v>
-      </c>
-      <c r="C16" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17004,11 +16991,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z918"/>
+  <dimension ref="A1:Z909"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17520,6 +17507,9 @@
       <c r="D17" t="s">
         <v>571</v>
       </c>
+      <c r="F17" t="s">
+        <v>1146</v>
+      </c>
       <c r="J17" t="s">
         <v>219</v>
       </c>
@@ -31326,6 +31316,9 @@
       <c r="D536" t="s">
         <v>571</v>
       </c>
+      <c r="F536" t="s">
+        <v>1146</v>
+      </c>
       <c r="J536" t="s">
         <v>219</v>
       </c>
@@ -32729,6 +32722,9 @@
       <c r="D588" t="s">
         <v>571</v>
       </c>
+      <c r="F588" t="s">
+        <v>1146</v>
+      </c>
       <c r="J588" t="s">
         <v>219</v>
       </c>
@@ -34152,6 +34148,9 @@
       <c r="D641" t="s">
         <v>571</v>
       </c>
+      <c r="F641" t="s">
+        <v>1146</v>
+      </c>
       <c r="J641" t="s">
         <v>219</v>
       </c>
@@ -34912,6 +34911,9 @@
       <c r="D670" t="s">
         <v>571</v>
       </c>
+      <c r="F670" t="s">
+        <v>1146</v>
+      </c>
       <c r="J670" t="s">
         <v>219</v>
       </c>
@@ -35809,6 +35811,9 @@
       <c r="D703" t="s">
         <v>571</v>
       </c>
+      <c r="F703" t="s">
+        <v>1146</v>
+      </c>
       <c r="J703" t="s">
         <v>219</v>
       </c>
@@ -37111,6 +37116,9 @@
       <c r="D751" t="s">
         <v>571</v>
       </c>
+      <c r="F751" t="s">
+        <v>1146</v>
+      </c>
       <c r="J751" t="s">
         <v>219</v>
       </c>
@@ -37713,11 +37721,14 @@
     </row>
     <row r="774" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B774" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="D774" t="s">
         <v>571</v>
       </c>
+      <c r="F774" t="s">
+        <v>1146</v>
+      </c>
       <c r="J774" t="s">
         <v>219</v>
       </c>
@@ -37739,13 +37750,13 @@
     </row>
     <row r="775" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B775" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="D775" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J775" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="M775" t="s">
         <v>134</v>
@@ -37765,13 +37776,13 @@
     </row>
     <row r="776" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B776" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="D776" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="J776" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="M776" t="s">
         <v>134</v>
@@ -37791,13 +37802,13 @@
     </row>
     <row r="777" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B777" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="D777" t="s">
-        <v>884</v>
+        <v>720</v>
       </c>
       <c r="J777" t="s">
-        <v>478</v>
+        <v>170</v>
       </c>
       <c r="M777" t="s">
         <v>134</v>
@@ -37817,22 +37828,19 @@
     </row>
     <row r="778" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B778" t="s">
-        <v>604</v>
+        <v>98</v>
       </c>
       <c r="D778" t="s">
-        <v>858</v>
+        <v>754</v>
       </c>
       <c r="J778" t="s">
-        <v>252</v>
+        <v>493</v>
       </c>
       <c r="M778" t="s">
         <v>134</v>
       </c>
       <c r="N778" t="s">
         <v>134</v>
-      </c>
-      <c r="O778" t="b">
-        <v>0</v>
       </c>
       <c r="Q778">
         <v>0</v>
@@ -37846,13 +37854,13 @@
     </row>
     <row r="779" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B779" t="s">
-        <v>605</v>
+        <v>98</v>
       </c>
       <c r="D779" t="s">
-        <v>571</v>
+        <v>755</v>
       </c>
       <c r="J779" t="s">
-        <v>219</v>
+        <v>494</v>
       </c>
       <c r="M779" t="s">
         <v>134</v>
@@ -37872,13 +37880,13 @@
     </row>
     <row r="780" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B780" t="s">
-        <v>605</v>
+        <v>98</v>
       </c>
       <c r="D780" t="s">
-        <v>643</v>
+        <v>756</v>
       </c>
       <c r="J780" t="s">
-        <v>81</v>
+        <v>495</v>
       </c>
       <c r="M780" t="s">
         <v>134</v>
@@ -37898,13 +37906,13 @@
     </row>
     <row r="781" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B781" t="s">
-        <v>605</v>
+        <v>98</v>
       </c>
       <c r="D781" t="s">
-        <v>642</v>
+        <v>757</v>
       </c>
       <c r="J781" t="s">
-        <v>73</v>
+        <v>499</v>
       </c>
       <c r="M781" t="s">
         <v>134</v>
@@ -37924,13 +37932,13 @@
     </row>
     <row r="782" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B782" t="s">
-        <v>605</v>
+        <v>98</v>
       </c>
       <c r="D782" t="s">
-        <v>880</v>
+        <v>758</v>
       </c>
       <c r="J782" t="s">
-        <v>465</v>
+        <v>500</v>
       </c>
       <c r="M782" t="s">
         <v>134</v>
@@ -37953,10 +37961,10 @@
         <v>98</v>
       </c>
       <c r="D783" t="s">
-        <v>571</v>
+        <v>922</v>
       </c>
       <c r="J783" t="s">
-        <v>219</v>
+        <v>497</v>
       </c>
       <c r="M783" t="s">
         <v>134</v>
@@ -37976,13 +37984,13 @@
     </row>
     <row r="784" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B784" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D784" t="s">
-        <v>642</v>
+        <v>982</v>
       </c>
       <c r="J784" t="s">
-        <v>73</v>
+        <v>560</v>
       </c>
       <c r="M784" t="s">
         <v>134</v>
@@ -38002,13 +38010,13 @@
     </row>
     <row r="785" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B785" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D785" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="J785" t="s">
-        <v>81</v>
+        <v>562</v>
       </c>
       <c r="M785" t="s">
         <v>134</v>
@@ -38028,13 +38036,13 @@
     </row>
     <row r="786" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B786" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D786" t="s">
-        <v>720</v>
+        <v>984</v>
       </c>
       <c r="J786" t="s">
-        <v>170</v>
+        <v>565</v>
       </c>
       <c r="M786" t="s">
         <v>134</v>
@@ -38054,13 +38062,13 @@
     </row>
     <row r="787" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B787" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D787" t="s">
-        <v>754</v>
+        <v>957</v>
       </c>
       <c r="J787" t="s">
-        <v>493</v>
+        <v>564</v>
       </c>
       <c r="M787" t="s">
         <v>134</v>
@@ -38080,16 +38088,16 @@
     </row>
     <row r="788" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B788" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D788" t="s">
-        <v>755</v>
+        <v>983</v>
       </c>
       <c r="J788" t="s">
-        <v>494</v>
+        <v>561</v>
       </c>
       <c r="M788" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N788" t="s">
         <v>134</v>
@@ -38106,13 +38114,13 @@
     </row>
     <row r="789" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B789" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D789" t="s">
-        <v>756</v>
+        <v>632</v>
       </c>
       <c r="J789" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="M789" t="s">
         <v>134</v>
@@ -38132,13 +38140,13 @@
     </row>
     <row r="790" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B790" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D790" t="s">
-        <v>757</v>
+        <v>635</v>
       </c>
       <c r="J790" t="s">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="M790" t="s">
         <v>134</v>
@@ -38158,13 +38166,13 @@
     </row>
     <row r="791" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B791" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D791" t="s">
-        <v>758</v>
+        <v>633</v>
       </c>
       <c r="J791" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="M791" t="s">
         <v>134</v>
@@ -38184,13 +38192,13 @@
     </row>
     <row r="792" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B792" t="s">
-        <v>98</v>
+        <v>606</v>
       </c>
       <c r="D792" t="s">
-        <v>922</v>
+        <v>636</v>
       </c>
       <c r="J792" t="s">
-        <v>497</v>
+        <v>536</v>
       </c>
       <c r="M792" t="s">
         <v>134</v>
@@ -38213,10 +38221,10 @@
         <v>606</v>
       </c>
       <c r="D793" t="s">
-        <v>982</v>
+        <v>638</v>
       </c>
       <c r="J793" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M793" t="s">
         <v>134</v>
@@ -38239,10 +38247,10 @@
         <v>606</v>
       </c>
       <c r="D794" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="J794" t="s">
-        <v>562</v>
+        <v>537</v>
       </c>
       <c r="M794" t="s">
         <v>134</v>
@@ -38265,10 +38273,10 @@
         <v>606</v>
       </c>
       <c r="D795" t="s">
-        <v>984</v>
+        <v>634</v>
       </c>
       <c r="J795" t="s">
-        <v>565</v>
+        <v>534</v>
       </c>
       <c r="M795" t="s">
         <v>134</v>
@@ -38291,10 +38299,10 @@
         <v>606</v>
       </c>
       <c r="D796" t="s">
-        <v>957</v>
+        <v>646</v>
       </c>
       <c r="J796" t="s">
-        <v>564</v>
+        <v>512</v>
       </c>
       <c r="M796" t="s">
         <v>134</v>
@@ -38317,13 +38325,13 @@
         <v>606</v>
       </c>
       <c r="D797" t="s">
-        <v>983</v>
+        <v>645</v>
       </c>
       <c r="J797" t="s">
-        <v>561</v>
+        <v>511</v>
       </c>
       <c r="M797" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N797" t="s">
         <v>134</v>
@@ -38343,10 +38351,10 @@
         <v>606</v>
       </c>
       <c r="D798" t="s">
-        <v>632</v>
+        <v>566</v>
       </c>
       <c r="J798" t="s">
-        <v>532</v>
+        <v>148</v>
       </c>
       <c r="M798" t="s">
         <v>134</v>
@@ -38369,10 +38377,10 @@
         <v>606</v>
       </c>
       <c r="D799" t="s">
-        <v>635</v>
+        <v>651</v>
       </c>
       <c r="J799" t="s">
-        <v>535</v>
+        <v>152</v>
       </c>
       <c r="M799" t="s">
         <v>134</v>
@@ -38395,10 +38403,10 @@
         <v>606</v>
       </c>
       <c r="D800" t="s">
-        <v>633</v>
+        <v>658</v>
       </c>
       <c r="J800" t="s">
-        <v>533</v>
+        <v>251</v>
       </c>
       <c r="M800" t="s">
         <v>134</v>
@@ -38410,21 +38418,21 @@
         <v>0</v>
       </c>
       <c r="R800">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="W800">
         <v>0</v>
       </c>
     </row>
-    <row r="801" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="801" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B801" t="s">
         <v>606</v>
       </c>
       <c r="D801" t="s">
-        <v>636</v>
+        <v>660</v>
       </c>
       <c r="J801" t="s">
-        <v>536</v>
+        <v>260</v>
       </c>
       <c r="M801" t="s">
         <v>134</v>
@@ -38442,15 +38450,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="802" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="802" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B802" t="s">
         <v>606</v>
       </c>
       <c r="D802" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
       <c r="J802" t="s">
-        <v>538</v>
+        <v>324</v>
       </c>
       <c r="M802" t="s">
         <v>134</v>
@@ -38468,15 +38476,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="803" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="803" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B803" t="s">
         <v>606</v>
       </c>
       <c r="D803" t="s">
-        <v>637</v>
+        <v>674</v>
       </c>
       <c r="J803" t="s">
-        <v>537</v>
+        <v>326</v>
       </c>
       <c r="M803" t="s">
         <v>134</v>
@@ -38494,18 +38502,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="804" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="804" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B804" t="s">
         <v>606</v>
       </c>
       <c r="D804" t="s">
-        <v>634</v>
+        <v>696</v>
       </c>
       <c r="J804" t="s">
-        <v>534</v>
+        <v>350</v>
       </c>
       <c r="M804" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N804" t="s">
         <v>134</v>
@@ -38514,24 +38522,24 @@
         <v>0</v>
       </c>
       <c r="R804">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="W804">
         <v>0</v>
       </c>
     </row>
-    <row r="805" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="805" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B805" t="s">
         <v>606</v>
       </c>
       <c r="D805" t="s">
-        <v>646</v>
+        <v>715</v>
       </c>
       <c r="J805" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="M805" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N805" t="s">
         <v>134</v>
@@ -38546,15 +38554,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="806" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="806" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B806" t="s">
         <v>606</v>
       </c>
       <c r="D806" t="s">
-        <v>645</v>
+        <v>716</v>
       </c>
       <c r="J806" t="s">
-        <v>511</v>
+        <v>531</v>
       </c>
       <c r="M806" t="s">
         <v>134</v>
@@ -38572,15 +38580,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="807" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="807" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B807" t="s">
         <v>606</v>
       </c>
       <c r="D807" t="s">
-        <v>566</v>
+        <v>718</v>
       </c>
       <c r="J807" t="s">
-        <v>148</v>
+        <v>543</v>
       </c>
       <c r="M807" t="s">
         <v>134</v>
@@ -38598,15 +38606,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="808" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="808" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B808" t="s">
         <v>606</v>
       </c>
       <c r="D808" t="s">
-        <v>651</v>
+        <v>717</v>
       </c>
       <c r="J808" t="s">
-        <v>152</v>
+        <v>542</v>
       </c>
       <c r="M808" t="s">
         <v>134</v>
@@ -38624,18 +38632,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="809" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="809" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B809" t="s">
         <v>606</v>
       </c>
       <c r="D809" t="s">
-        <v>658</v>
+        <v>77</v>
       </c>
       <c r="J809" t="s">
-        <v>251</v>
+        <v>85</v>
       </c>
       <c r="M809" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N809" t="s">
         <v>134</v>
@@ -38644,24 +38652,24 @@
         <v>0</v>
       </c>
       <c r="R809">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="W809">
         <v>0</v>
       </c>
     </row>
-    <row r="810" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="810" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B810" t="s">
         <v>606</v>
       </c>
       <c r="D810" t="s">
-        <v>660</v>
+        <v>579</v>
       </c>
       <c r="J810" t="s">
-        <v>260</v>
+        <v>513</v>
       </c>
       <c r="M810" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N810" t="s">
         <v>134</v>
@@ -38676,18 +38684,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="811" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="811" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B811" t="s">
         <v>606</v>
       </c>
       <c r="D811" t="s">
-        <v>672</v>
+        <v>108</v>
       </c>
       <c r="J811" t="s">
-        <v>324</v>
+        <v>514</v>
       </c>
       <c r="M811" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N811" t="s">
         <v>134</v>
@@ -38702,15 +38710,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="812" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="812" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B812" t="s">
         <v>606</v>
       </c>
       <c r="D812" t="s">
-        <v>674</v>
+        <v>760</v>
       </c>
       <c r="J812" t="s">
-        <v>326</v>
+        <v>158</v>
       </c>
       <c r="M812" t="s">
         <v>134</v>
@@ -38725,21 +38733,21 @@
         <v>0</v>
       </c>
       <c r="W812">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="813" spans="2:23" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="813" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B813" t="s">
         <v>606</v>
       </c>
       <c r="D813" t="s">
-        <v>696</v>
+        <v>761</v>
       </c>
       <c r="J813" t="s">
-        <v>350</v>
+        <v>159</v>
       </c>
       <c r="M813" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N813" t="s">
         <v>134</v>
@@ -38748,24 +38756,24 @@
         <v>0</v>
       </c>
       <c r="R813">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W813">
         <v>0</v>
       </c>
     </row>
-    <row r="814" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="814" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B814" t="s">
         <v>606</v>
       </c>
       <c r="D814" t="s">
-        <v>715</v>
+        <v>817</v>
       </c>
       <c r="J814" t="s">
-        <v>530</v>
+        <v>256</v>
       </c>
       <c r="M814" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N814" t="s">
         <v>134</v>
@@ -38780,15 +38788,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="815" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="815" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B815" t="s">
         <v>606</v>
       </c>
       <c r="D815" t="s">
-        <v>716</v>
+        <v>827</v>
       </c>
       <c r="J815" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="M815" t="s">
         <v>134</v>
@@ -38802,19 +38810,31 @@
       <c r="R815">
         <v>0</v>
       </c>
+      <c r="V815">
+        <v>999999999999990</v>
+      </c>
       <c r="W815">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="816" spans="2:23" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="X815" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y815" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z815" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="816" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B816" t="s">
         <v>606</v>
       </c>
       <c r="D816" t="s">
-        <v>718</v>
+        <v>828</v>
       </c>
       <c r="J816" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="M816" t="s">
         <v>134</v>
@@ -38828,8 +38848,20 @@
       <c r="R816">
         <v>0</v>
       </c>
+      <c r="V816">
+        <v>999999999999990</v>
+      </c>
       <c r="W816">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="X816" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y816" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z816" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="817" spans="2:26" x14ac:dyDescent="0.2">
@@ -38837,13 +38869,13 @@
         <v>606</v>
       </c>
       <c r="D817" t="s">
-        <v>717</v>
+        <v>825</v>
       </c>
       <c r="J817" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="M817" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N817" t="s">
         <v>134</v>
@@ -38854,8 +38886,20 @@
       <c r="R817">
         <v>0</v>
       </c>
+      <c r="V817">
+        <v>999999999999990</v>
+      </c>
       <c r="W817">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="X817" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y817" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z817" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="818" spans="2:26" x14ac:dyDescent="0.2">
@@ -38863,10 +38907,10 @@
         <v>606</v>
       </c>
       <c r="D818" t="s">
-        <v>77</v>
+        <v>826</v>
       </c>
       <c r="J818" t="s">
-        <v>85</v>
+        <v>525</v>
       </c>
       <c r="M818" t="s">
         <v>104</v>
@@ -38880,8 +38924,20 @@
       <c r="R818">
         <v>0</v>
       </c>
+      <c r="V818">
+        <v>999999999999990</v>
+      </c>
       <c r="W818">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="X818" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y818" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z818" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="819" spans="2:26" x14ac:dyDescent="0.2">
@@ -38889,13 +38945,13 @@
         <v>606</v>
       </c>
       <c r="D819" t="s">
-        <v>579</v>
+        <v>888</v>
       </c>
       <c r="J819" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="M819" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N819" t="s">
         <v>134</v>
@@ -38906,8 +38962,20 @@
       <c r="R819">
         <v>0</v>
       </c>
+      <c r="V819">
+        <v>999999999999990</v>
+      </c>
       <c r="W819">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="X819" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y819" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z819" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="820" spans="2:26" x14ac:dyDescent="0.2">
@@ -38915,16 +38983,16 @@
         <v>606</v>
       </c>
       <c r="D820" t="s">
-        <v>108</v>
+        <v>847</v>
       </c>
       <c r="J820" t="s">
-        <v>514</v>
+        <v>187</v>
       </c>
       <c r="M820" t="s">
         <v>104</v>
       </c>
       <c r="N820" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="Q820">
         <v>0</v>
@@ -38941,13 +39009,13 @@
         <v>606</v>
       </c>
       <c r="D821" t="s">
-        <v>760</v>
+        <v>604</v>
       </c>
       <c r="J821" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="M821" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N821" t="s">
         <v>134</v>
@@ -38959,7 +39027,7 @@
         <v>0</v>
       </c>
       <c r="W821">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="822" spans="2:26" x14ac:dyDescent="0.2">
@@ -38967,13 +39035,13 @@
         <v>606</v>
       </c>
       <c r="D822" t="s">
-        <v>761</v>
+        <v>889</v>
       </c>
       <c r="J822" t="s">
-        <v>159</v>
+        <v>552</v>
       </c>
       <c r="M822" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N822" t="s">
         <v>134</v>
@@ -38993,16 +39061,19 @@
         <v>606</v>
       </c>
       <c r="D823" t="s">
-        <v>817</v>
+        <v>867</v>
       </c>
       <c r="J823" t="s">
-        <v>256</v>
+        <v>348</v>
       </c>
       <c r="M823" t="s">
         <v>134</v>
       </c>
       <c r="N823" t="s">
         <v>134</v>
+      </c>
+      <c r="O823">
+        <v>1</v>
       </c>
       <c r="Q823">
         <v>0</v>
@@ -39019,10 +39090,10 @@
         <v>606</v>
       </c>
       <c r="D824" t="s">
-        <v>827</v>
+        <v>887</v>
       </c>
       <c r="J824" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="M824" t="s">
         <v>134</v>
@@ -39046,7 +39117,7 @@
         <v>39</v>
       </c>
       <c r="Y824" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="Z824" t="s">
         <v>196</v>
@@ -39057,13 +39128,13 @@
         <v>606</v>
       </c>
       <c r="D825" t="s">
-        <v>828</v>
+        <v>904</v>
       </c>
       <c r="J825" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
       <c r="M825" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N825" t="s">
         <v>134</v>
@@ -39074,20 +39145,8 @@
       <c r="R825">
         <v>0</v>
       </c>
-      <c r="V825">
-        <v>999999999999990</v>
-      </c>
       <c r="W825">
-        <v>2</v>
-      </c>
-      <c r="X825" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y825" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z825" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="826" spans="2:26" x14ac:dyDescent="0.2">
@@ -39095,13 +39154,13 @@
         <v>606</v>
       </c>
       <c r="D826" t="s">
-        <v>825</v>
+        <v>927</v>
       </c>
       <c r="J826" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="M826" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N826" t="s">
         <v>134</v>
@@ -39112,20 +39171,8 @@
       <c r="R826">
         <v>0</v>
       </c>
-      <c r="V826">
-        <v>999999999999990</v>
-      </c>
       <c r="W826">
-        <v>2</v>
-      </c>
-      <c r="X826" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y826" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z826" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="827" spans="2:26" x14ac:dyDescent="0.2">
@@ -39133,13 +39180,13 @@
         <v>606</v>
       </c>
       <c r="D827" t="s">
-        <v>826</v>
+        <v>931</v>
       </c>
       <c r="J827" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="M827" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N827" t="s">
         <v>134</v>
@@ -39150,20 +39197,8 @@
       <c r="R827">
         <v>0</v>
       </c>
-      <c r="V827">
-        <v>999999999999990</v>
-      </c>
       <c r="W827">
-        <v>2</v>
-      </c>
-      <c r="X827" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y827" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z827" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="828" spans="2:26" x14ac:dyDescent="0.2">
@@ -39171,10 +39206,10 @@
         <v>606</v>
       </c>
       <c r="D828" t="s">
-        <v>888</v>
+        <v>933</v>
       </c>
       <c r="J828" t="s">
-        <v>529</v>
+        <v>548</v>
       </c>
       <c r="M828" t="s">
         <v>134</v>
@@ -39188,20 +39223,11 @@
       <c r="R828">
         <v>0</v>
       </c>
-      <c r="V828">
-        <v>999999999999990</v>
+      <c r="T828">
+        <v>0</v>
       </c>
       <c r="W828">
-        <v>2</v>
-      </c>
-      <c r="X828" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y828" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z828" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="829" spans="2:26" x14ac:dyDescent="0.2">
@@ -39209,16 +39235,16 @@
         <v>606</v>
       </c>
       <c r="D829" t="s">
-        <v>847</v>
+        <v>925</v>
       </c>
       <c r="J829" t="s">
-        <v>187</v>
+        <v>517</v>
       </c>
       <c r="M829" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N829" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="Q829">
         <v>0</v>
@@ -39235,13 +39261,13 @@
         <v>606</v>
       </c>
       <c r="D830" t="s">
-        <v>604</v>
+        <v>929</v>
       </c>
       <c r="J830" t="s">
-        <v>125</v>
+        <v>521</v>
       </c>
       <c r="M830" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N830" t="s">
         <v>134</v>
@@ -39261,16 +39287,19 @@
         <v>606</v>
       </c>
       <c r="D831" t="s">
-        <v>889</v>
+        <v>926</v>
       </c>
       <c r="J831" t="s">
-        <v>552</v>
+        <v>518</v>
       </c>
       <c r="M831" t="s">
         <v>104</v>
       </c>
       <c r="N831" t="s">
         <v>134</v>
+      </c>
+      <c r="O831">
+        <v>128</v>
       </c>
       <c r="Q831">
         <v>0</v>
@@ -39287,10 +39316,10 @@
         <v>606</v>
       </c>
       <c r="D832" t="s">
-        <v>867</v>
+        <v>930</v>
       </c>
       <c r="J832" t="s">
-        <v>348</v>
+        <v>522</v>
       </c>
       <c r="M832" t="s">
         <v>134</v>
@@ -39298,9 +39327,6 @@
       <c r="N832" t="s">
         <v>134</v>
       </c>
-      <c r="O832">
-        <v>1</v>
-      </c>
       <c r="Q832">
         <v>0</v>
       </c>
@@ -39311,15 +39337,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="833" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="833" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B833" t="s">
         <v>606</v>
       </c>
       <c r="D833" t="s">
-        <v>887</v>
+        <v>932</v>
       </c>
       <c r="J833" t="s">
-        <v>528</v>
+        <v>547</v>
       </c>
       <c r="M833" t="s">
         <v>134</v>
@@ -39327,37 +39353,31 @@
       <c r="N833" t="s">
         <v>134</v>
       </c>
+      <c r="O833">
+        <v>1</v>
+      </c>
       <c r="Q833">
         <v>0</v>
       </c>
       <c r="R833">
         <v>0</v>
       </c>
-      <c r="V833">
-        <v>999999999999990</v>
+      <c r="T833">
+        <v>0</v>
       </c>
       <c r="W833">
-        <v>2</v>
-      </c>
-      <c r="X833" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y833" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z833" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="834" spans="2:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B834" t="s">
         <v>606</v>
       </c>
       <c r="D834" t="s">
-        <v>904</v>
+        <v>924</v>
       </c>
       <c r="J834" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="M834" t="s">
         <v>104</v>
@@ -39365,6 +39385,9 @@
       <c r="N834" t="s">
         <v>134</v>
       </c>
+      <c r="O834">
+        <v>128</v>
+      </c>
       <c r="Q834">
         <v>0</v>
       </c>
@@ -39375,18 +39398,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="835" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="835" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B835" t="s">
         <v>606</v>
       </c>
       <c r="D835" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="J835" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="M835" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N835" t="s">
         <v>134</v>
@@ -39401,18 +39424,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="836" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="836" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B836" t="s">
         <v>606</v>
       </c>
       <c r="D836" t="s">
-        <v>931</v>
+        <v>79</v>
       </c>
       <c r="J836" t="s">
-        <v>523</v>
+        <v>88</v>
       </c>
       <c r="M836" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N836" t="s">
         <v>134</v>
@@ -39421,24 +39444,24 @@
         <v>0</v>
       </c>
       <c r="R836">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W836">
         <v>0</v>
       </c>
     </row>
-    <row r="837" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="837" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B837" t="s">
         <v>606</v>
       </c>
       <c r="D837" t="s">
-        <v>933</v>
+        <v>923</v>
       </c>
       <c r="J837" t="s">
-        <v>548</v>
+        <v>515</v>
       </c>
       <c r="M837" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N837" t="s">
         <v>134</v>
@@ -39447,24 +39470,21 @@
         <v>0</v>
       </c>
       <c r="R837">
-        <v>0</v>
-      </c>
-      <c r="T837">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W837">
         <v>0</v>
       </c>
     </row>
-    <row r="838" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="838" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B838" t="s">
         <v>606</v>
       </c>
       <c r="D838" t="s">
-        <v>925</v>
+        <v>956</v>
       </c>
       <c r="J838" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="M838" t="s">
         <v>134</v>
@@ -39473,27 +39493,27 @@
         <v>134</v>
       </c>
       <c r="Q838">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R838">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="W838">
         <v>0</v>
       </c>
     </row>
-    <row r="839" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="839" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B839" t="s">
         <v>606</v>
       </c>
       <c r="D839" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="J839" t="s">
-        <v>521</v>
+        <v>207</v>
       </c>
       <c r="M839" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N839" t="s">
         <v>134</v>
@@ -39508,25 +39528,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="840" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="840" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B840" t="s">
         <v>606</v>
       </c>
       <c r="D840" t="s">
-        <v>926</v>
+        <v>937</v>
       </c>
       <c r="J840" t="s">
-        <v>518</v>
+        <v>213</v>
       </c>
       <c r="M840" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N840" t="s">
         <v>134</v>
       </c>
-      <c r="O840">
-        <v>128</v>
-      </c>
       <c r="Q840">
         <v>0</v>
       </c>
@@ -39537,22 +39554,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="841" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="841" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B841" t="s">
         <v>606</v>
       </c>
       <c r="D841" t="s">
-        <v>930</v>
+        <v>943</v>
       </c>
       <c r="J841" t="s">
-        <v>522</v>
+        <v>89</v>
       </c>
       <c r="M841" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N841" t="s">
         <v>134</v>
       </c>
+      <c r="O841">
+        <v>1</v>
+      </c>
       <c r="Q841">
         <v>0</v>
       </c>
@@ -39563,24 +39583,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="842" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="842" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B842" t="s">
         <v>606</v>
       </c>
       <c r="D842" t="s">
-        <v>932</v>
+        <v>951</v>
       </c>
       <c r="J842" t="s">
-        <v>547</v>
+        <v>359</v>
       </c>
       <c r="M842" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N842" t="s">
-        <v>134</v>
-      </c>
-      <c r="O842">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="Q842">
         <v>0</v>
@@ -39588,51 +39605,45 @@
       <c r="R842">
         <v>0</v>
       </c>
-      <c r="T842">
-        <v>0</v>
-      </c>
       <c r="W842">
         <v>0</v>
       </c>
     </row>
-    <row r="843" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="843" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B843" t="s">
         <v>606</v>
       </c>
       <c r="D843" t="s">
-        <v>924</v>
+        <v>955</v>
       </c>
       <c r="J843" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="M843" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N843" t="s">
         <v>134</v>
       </c>
-      <c r="O843">
-        <v>128</v>
-      </c>
       <c r="Q843">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R843">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="W843">
         <v>0</v>
       </c>
     </row>
-    <row r="844" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="844" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B844" t="s">
         <v>606</v>
       </c>
       <c r="D844" t="s">
-        <v>928</v>
+        <v>973</v>
       </c>
       <c r="J844" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="M844" t="s">
         <v>104</v>
@@ -39650,15 +39661,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="845" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="845" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B845" t="s">
         <v>606</v>
       </c>
       <c r="D845" t="s">
-        <v>79</v>
+        <v>975</v>
       </c>
       <c r="J845" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="M845" t="s">
         <v>104</v>
@@ -39666,28 +39677,31 @@
       <c r="N845" t="s">
         <v>134</v>
       </c>
+      <c r="O845" t="s">
+        <v>594</v>
+      </c>
       <c r="Q845">
         <v>0</v>
       </c>
       <c r="R845">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W845">
         <v>0</v>
       </c>
     </row>
-    <row r="846" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="846" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B846" t="s">
         <v>606</v>
       </c>
       <c r="D846" t="s">
-        <v>923</v>
+        <v>977</v>
       </c>
       <c r="J846" t="s">
-        <v>515</v>
+        <v>544</v>
       </c>
       <c r="M846" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N846" t="s">
         <v>134</v>
@@ -39696,47 +39710,47 @@
         <v>0</v>
       </c>
       <c r="R846">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W846">
         <v>0</v>
       </c>
     </row>
-    <row r="847" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="847" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B847" t="s">
         <v>606</v>
       </c>
       <c r="D847" t="s">
-        <v>956</v>
+        <v>976</v>
       </c>
       <c r="J847" t="s">
-        <v>540</v>
+        <v>508</v>
       </c>
       <c r="M847" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N847" t="s">
         <v>134</v>
       </c>
       <c r="Q847">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R847">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="W847">
         <v>0</v>
       </c>
     </row>
-    <row r="848" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="848" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B848" t="s">
         <v>606</v>
       </c>
       <c r="D848" t="s">
-        <v>936</v>
+        <v>974</v>
       </c>
       <c r="J848" t="s">
-        <v>207</v>
+        <v>507</v>
       </c>
       <c r="M848" t="s">
         <v>104</v>
@@ -39759,13 +39773,13 @@
         <v>606</v>
       </c>
       <c r="D849" t="s">
-        <v>937</v>
+        <v>979</v>
       </c>
       <c r="J849" t="s">
-        <v>213</v>
+        <v>546</v>
       </c>
       <c r="M849" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N849" t="s">
         <v>134</v>
@@ -39785,19 +39799,16 @@
         <v>606</v>
       </c>
       <c r="D850" t="s">
-        <v>943</v>
+        <v>76</v>
       </c>
       <c r="J850" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="M850" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N850" t="s">
         <v>134</v>
-      </c>
-      <c r="O850">
-        <v>1</v>
       </c>
       <c r="Q850">
         <v>0</v>
@@ -39814,16 +39825,16 @@
         <v>606</v>
       </c>
       <c r="D851" t="s">
-        <v>951</v>
+        <v>978</v>
       </c>
       <c r="J851" t="s">
-        <v>359</v>
+        <v>545</v>
       </c>
       <c r="M851" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N851" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="Q851">
         <v>0</v>
@@ -39840,22 +39851,22 @@
         <v>606</v>
       </c>
       <c r="D852" t="s">
-        <v>955</v>
+        <v>647</v>
       </c>
       <c r="J852" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="M852" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N852" t="s">
         <v>134</v>
       </c>
       <c r="Q852">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R852">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="W852">
         <v>0</v>
@@ -39866,13 +39877,13 @@
         <v>606</v>
       </c>
       <c r="D853" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
       <c r="J853" t="s">
-        <v>506</v>
+        <v>549</v>
       </c>
       <c r="M853" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N853" t="s">
         <v>134</v>
@@ -39892,19 +39903,16 @@
         <v>606</v>
       </c>
       <c r="D854" t="s">
-        <v>975</v>
+        <v>981</v>
       </c>
       <c r="J854" t="s">
-        <v>105</v>
+        <v>550</v>
       </c>
       <c r="M854" t="s">
         <v>104</v>
       </c>
       <c r="N854" t="s">
         <v>134</v>
-      </c>
-      <c r="O854" t="s">
-        <v>594</v>
       </c>
       <c r="Q854">
         <v>0</v>
@@ -39921,16 +39929,19 @@
         <v>606</v>
       </c>
       <c r="D855" t="s">
-        <v>977</v>
+        <v>580</v>
       </c>
       <c r="J855" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="M855" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="N855" t="s">
         <v>134</v>
+      </c>
+      <c r="O855" t="s">
+        <v>596</v>
       </c>
       <c r="Q855">
         <v>0</v>
@@ -39947,10 +39958,10 @@
         <v>606</v>
       </c>
       <c r="D856" t="s">
-        <v>976</v>
+        <v>747</v>
       </c>
       <c r="J856" t="s">
-        <v>508</v>
+        <v>553</v>
       </c>
       <c r="M856" t="s">
         <v>104</v>
@@ -39973,13 +39984,13 @@
         <v>606</v>
       </c>
       <c r="D857" t="s">
-        <v>974</v>
+        <v>781</v>
       </c>
       <c r="J857" t="s">
-        <v>507</v>
+        <v>289</v>
       </c>
       <c r="M857" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="N857" t="s">
         <v>134</v>
@@ -39996,511 +40007,346 @@
     </row>
     <row r="858" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B858" t="s">
-        <v>606</v>
-      </c>
-      <c r="D858" t="s">
-        <v>979</v>
-      </c>
-      <c r="J858" t="s">
-        <v>546</v>
-      </c>
-      <c r="M858" t="s">
-        <v>104</v>
-      </c>
-      <c r="N858" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q858">
-        <v>0</v>
-      </c>
-      <c r="R858">
-        <v>0</v>
-      </c>
-      <c r="W858">
-        <v>0</v>
+        <v>600</v>
+      </c>
+      <c r="E858" t="s">
+        <v>992</v>
       </c>
     </row>
     <row r="859" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B859" t="s">
-        <v>606</v>
-      </c>
-      <c r="D859" t="s">
-        <v>76</v>
-      </c>
-      <c r="J859" t="s">
-        <v>82</v>
-      </c>
-      <c r="M859" t="s">
-        <v>134</v>
-      </c>
-      <c r="N859" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q859">
-        <v>0</v>
-      </c>
-      <c r="R859">
-        <v>0</v>
-      </c>
-      <c r="W859">
-        <v>0</v>
+        <v>602</v>
+      </c>
+      <c r="E859" t="s">
+        <v>993</v>
       </c>
     </row>
     <row r="860" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B860" t="s">
-        <v>606</v>
-      </c>
-      <c r="D860" t="s">
-        <v>978</v>
-      </c>
-      <c r="J860" t="s">
-        <v>545</v>
-      </c>
-      <c r="M860" t="s">
-        <v>134</v>
-      </c>
-      <c r="N860" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q860">
-        <v>0</v>
-      </c>
-      <c r="R860">
-        <v>0</v>
-      </c>
-      <c r="W860">
-        <v>0</v>
+        <v>598</v>
+      </c>
+      <c r="E860" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="861" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B861" t="s">
-        <v>606</v>
-      </c>
-      <c r="D861" t="s">
-        <v>647</v>
-      </c>
-      <c r="J861" t="s">
-        <v>541</v>
-      </c>
-      <c r="M861" t="s">
-        <v>104</v>
-      </c>
-      <c r="N861" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q861">
-        <v>0</v>
-      </c>
-      <c r="R861">
-        <v>0</v>
-      </c>
-      <c r="W861">
-        <v>0</v>
+        <v>598</v>
+      </c>
+      <c r="E861" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="862" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B862" t="s">
-        <v>606</v>
-      </c>
-      <c r="D862" t="s">
-        <v>980</v>
-      </c>
-      <c r="J862" t="s">
-        <v>549</v>
-      </c>
-      <c r="M862" t="s">
-        <v>134</v>
-      </c>
-      <c r="N862" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q862">
-        <v>0</v>
-      </c>
-      <c r="R862">
-        <v>0</v>
-      </c>
-      <c r="W862">
-        <v>0</v>
+        <v>598</v>
+      </c>
+      <c r="E862" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="863" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B863" t="s">
-        <v>606</v>
-      </c>
-      <c r="D863" t="s">
-        <v>981</v>
-      </c>
-      <c r="J863" t="s">
-        <v>550</v>
-      </c>
-      <c r="M863" t="s">
-        <v>104</v>
-      </c>
-      <c r="N863" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q863">
-        <v>0</v>
-      </c>
-      <c r="R863">
-        <v>0</v>
-      </c>
-      <c r="W863">
-        <v>0</v>
+        <v>598</v>
+      </c>
+      <c r="E863" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="864" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B864" t="s">
-        <v>606</v>
-      </c>
-      <c r="D864" t="s">
-        <v>580</v>
-      </c>
-      <c r="J864" t="s">
-        <v>551</v>
-      </c>
-      <c r="M864" t="s">
-        <v>104</v>
-      </c>
-      <c r="N864" t="s">
-        <v>134</v>
-      </c>
-      <c r="O864" t="s">
-        <v>596</v>
-      </c>
-      <c r="Q864">
-        <v>0</v>
-      </c>
-      <c r="R864">
-        <v>0</v>
-      </c>
-      <c r="W864">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="865" spans="2:23" x14ac:dyDescent="0.2">
+        <v>601</v>
+      </c>
+      <c r="E864" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="865" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B865" t="s">
-        <v>606</v>
-      </c>
-      <c r="D865" t="s">
-        <v>747</v>
-      </c>
-      <c r="J865" t="s">
-        <v>553</v>
-      </c>
-      <c r="M865" t="s">
-        <v>104</v>
-      </c>
-      <c r="N865" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q865">
-        <v>0</v>
-      </c>
-      <c r="R865">
-        <v>0</v>
-      </c>
-      <c r="W865">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="866" spans="2:23" x14ac:dyDescent="0.2">
+        <v>601</v>
+      </c>
+      <c r="E865" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="866" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B866" t="s">
-        <v>606</v>
-      </c>
-      <c r="D866" t="s">
-        <v>781</v>
-      </c>
-      <c r="J866" t="s">
-        <v>289</v>
-      </c>
-      <c r="M866" t="s">
-        <v>134</v>
-      </c>
-      <c r="N866" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q866">
-        <v>0</v>
-      </c>
-      <c r="R866">
-        <v>0</v>
-      </c>
-      <c r="W866">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="867" spans="2:23" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E866" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="867" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B867" t="s">
+        <v>118</v>
+      </c>
+      <c r="E867" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="868" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B868" t="s">
         <v>600</v>
       </c>
-      <c r="E867" t="s">
+      <c r="E868" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="869" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B869" t="s">
+        <v>601</v>
+      </c>
+      <c r="E869" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="870" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B870" t="s">
+        <v>114</v>
+      </c>
+      <c r="E870" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="871" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B871" t="s">
+        <v>599</v>
+      </c>
+      <c r="E871" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="872" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B872" t="s">
+        <v>29</v>
+      </c>
+      <c r="E872" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="873" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B873" t="s">
+        <v>118</v>
+      </c>
+      <c r="E873" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="874" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B874" t="s">
+        <v>600</v>
+      </c>
+      <c r="E874" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="875" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C875" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="868" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B868" t="s">
-        <v>602</v>
-      </c>
-      <c r="E868" t="s">
+      <c r="D875" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="876" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C876" t="s">
+        <v>992</v>
+      </c>
+      <c r="D876" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="877" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C877" t="s">
+        <v>998</v>
+      </c>
+      <c r="D877" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="878" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C878" t="s">
+        <v>998</v>
+      </c>
+      <c r="D878" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="879" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C879" t="s">
+        <v>998</v>
+      </c>
+      <c r="D879" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="880" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C880" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="869" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B869" t="s">
-        <v>598</v>
-      </c>
-      <c r="E869" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="870" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B870" t="s">
-        <v>598</v>
-      </c>
-      <c r="E870" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="871" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B871" t="s">
-        <v>598</v>
-      </c>
-      <c r="E871" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="872" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B872" t="s">
-        <v>598</v>
-      </c>
-      <c r="E872" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="873" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B873" t="s">
-        <v>601</v>
-      </c>
-      <c r="E873" t="s">
+      <c r="D880" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="881" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C881" t="s">
+        <v>993</v>
+      </c>
+      <c r="D881" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="882" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C882" t="s">
+        <v>993</v>
+      </c>
+      <c r="D882" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="883" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C883" t="s">
+        <v>993</v>
+      </c>
+      <c r="D883" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="884" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C884" t="s">
         <v>995</v>
-      </c>
-    </row>
-    <row r="874" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B874" t="s">
-        <v>601</v>
-      </c>
-      <c r="E874" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="875" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B875" t="s">
-        <v>29</v>
-      </c>
-      <c r="E875" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="876" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B876" t="s">
-        <v>118</v>
-      </c>
-      <c r="E876" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="877" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B877" t="s">
-        <v>600</v>
-      </c>
-      <c r="E877" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="878" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B878" t="s">
-        <v>601</v>
-      </c>
-      <c r="E878" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="879" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B879" t="s">
-        <v>114</v>
-      </c>
-      <c r="E879" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="880" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B880" t="s">
-        <v>599</v>
-      </c>
-      <c r="E880" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="881" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B881" t="s">
-        <v>29</v>
-      </c>
-      <c r="E881" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="882" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B882" t="s">
-        <v>118</v>
-      </c>
-      <c r="E882" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="883" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B883" t="s">
-        <v>600</v>
-      </c>
-      <c r="E883" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="884" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C884" t="s">
-        <v>992</v>
       </c>
       <c r="D884" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="885" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="885" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C885" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
       <c r="D885" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="886" spans="2:5" x14ac:dyDescent="0.2">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="886" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C886" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D886" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="887" spans="2:5" x14ac:dyDescent="0.2">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="887" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C887" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D887" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="888" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="888" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C888" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D888" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="889" spans="2:5" x14ac:dyDescent="0.2">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="889" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C889" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="D889" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="890" spans="2:5" x14ac:dyDescent="0.2">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="890" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C890" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="D890" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="891" spans="2:5" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="891" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C891" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="D891" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="892" spans="2:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="892" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C892" t="s">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c r="D892" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="893" spans="2:5" x14ac:dyDescent="0.2">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="893" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C893" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="D893" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="894" spans="2:5" x14ac:dyDescent="0.2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="894" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C894" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D894" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="895" spans="2:5" x14ac:dyDescent="0.2">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="895" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C895" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D895" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="896" spans="2:5" x14ac:dyDescent="0.2">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="896" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C896" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D896" t="s">
-        <v>643</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="897" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C897" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D897" t="s">
-        <v>884</v>
+        <v>79</v>
       </c>
     </row>
     <row r="898" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C898" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="D898" t="s">
-        <v>597</v>
+        <v>923</v>
       </c>
     </row>
     <row r="899" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C899" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="D899" t="s">
-        <v>120</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="900" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C900" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="D900" t="s">
-        <v>98</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="901" spans="3:4" x14ac:dyDescent="0.2">
@@ -40508,7 +40354,7 @@
         <v>997</v>
       </c>
       <c r="D901" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="902" spans="3:4" x14ac:dyDescent="0.2">
@@ -40516,7 +40362,7 @@
         <v>997</v>
       </c>
       <c r="D902" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="903" spans="3:4" x14ac:dyDescent="0.2">
@@ -40524,7 +40370,7 @@
         <v>997</v>
       </c>
       <c r="D903" t="s">
-        <v>597</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="904" spans="3:4" x14ac:dyDescent="0.2">
@@ -40532,7 +40378,7 @@
         <v>997</v>
       </c>
       <c r="D904" t="s">
-        <v>946</v>
+        <v>78</v>
       </c>
     </row>
     <row r="905" spans="3:4" x14ac:dyDescent="0.2">
@@ -40540,7 +40386,7 @@
         <v>997</v>
       </c>
       <c r="D905" t="s">
-        <v>1006</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="906" spans="3:4" x14ac:dyDescent="0.2">
@@ -40548,7 +40394,7 @@
         <v>997</v>
       </c>
       <c r="D906" t="s">
-        <v>79</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="907" spans="3:4" x14ac:dyDescent="0.2">
@@ -40556,7 +40402,7 @@
         <v>997</v>
       </c>
       <c r="D907" t="s">
-        <v>923</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="908" spans="3:4" x14ac:dyDescent="0.2">
@@ -40564,7 +40410,7 @@
         <v>997</v>
       </c>
       <c r="D908" t="s">
-        <v>1007</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="909" spans="3:4" x14ac:dyDescent="0.2">
@@ -40572,83 +40418,11 @@
         <v>997</v>
       </c>
       <c r="D909" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="910" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C910" t="s">
-        <v>997</v>
-      </c>
-      <c r="D910" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="911" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C911" t="s">
-        <v>997</v>
-      </c>
-      <c r="D911" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="912" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C912" t="s">
-        <v>997</v>
-      </c>
-      <c r="D912" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="913" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C913" t="s">
-        <v>997</v>
-      </c>
-      <c r="D913" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="914" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C914" t="s">
-        <v>997</v>
-      </c>
-      <c r="D914" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="915" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C915" t="s">
-        <v>997</v>
-      </c>
-      <c r="D915" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="916" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C916" t="s">
-        <v>997</v>
-      </c>
-      <c r="D916" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="917" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C917" t="s">
-        <v>997</v>
-      </c>
-      <c r="D917" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="918" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C918" t="s">
-        <v>997</v>
-      </c>
-      <c r="D918" t="s">
         <v>1016</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z918"/>
+  <autoFilter ref="A1:Z909"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>